<commit_message>
Ver1.2.0: Update sch and bom
</commit_message>
<xml_diff>
--- a/03_BOM/LASERDIODE_BOM_V1.2.0.xlsx
+++ b/03_BOM/LASERDIODE_BOM_V1.2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Altium\NANORACK\LASERDIODE V1.2.0\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1370F4-28C6-42ED-B42E-F107892676ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD035AEB-1379-497E-A550-45C72EB96074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LASER_BOM" sheetId="5" r:id="rId1"/>
@@ -659,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -701,7 +701,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -920,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1678,7 +1677,7 @@
       <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="14.25" customHeight="1">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>153</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -1693,9 +1692,9 @@
         <v>150</v>
       </c>
       <c r="G31" s="30">
-        <v>4</v>
-      </c>
-      <c r="H31" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="H31" s="31" t="s">
         <v>154</v>
       </c>
       <c r="I31" s="3"/>

</xml_diff>